<commit_message>
Registration final and login
</commit_message>
<xml_diff>
--- a/Users.xlsx
+++ b/Users.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\slava\Desktop\wiki\Wiki\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0999960A-8597-454C-ABAD-9EB8E10E0051}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27780" windowHeight="16200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -18,8 +24,31 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+  <si>
+    <t>penismaster</t>
+  </si>
+  <si>
+    <t>5fa285e1bebe0a6623e33afc04a1fbd5</t>
+  </si>
+  <si>
+    <t>wdf</t>
+  </si>
+  <si>
+    <t>d1c364f4b712dc6c804c2b773de76d97</t>
+  </si>
+  <si>
+    <t>penis</t>
+  </si>
+  <si>
+    <t>46dc363a5e754c6781f8889094b288c4</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -53,7 +82,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -330,13 +359,46 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A2:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>123</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
LOGIN FINALLY DONE SADFJIOJSKDFOPDSFL:FDS
</commit_message>
<xml_diff>
--- a/Users.xlsx
+++ b/Users.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\slava\Desktop\wiki\Wiki\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0999960A-8597-454C-ABAD-9EB8E10E0051}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09D960EF-4C4A-402A-AD49-753A649217BB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="27780" windowHeight="16200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,24 +25,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>penismaster</t>
+    <t>asd</t>
   </si>
   <si>
     <t>5fa285e1bebe0a6623e33afc04a1fbd5</t>
-  </si>
-  <si>
-    <t>wdf</t>
-  </si>
-  <si>
-    <t>d1c364f4b712dc6c804c2b773de76d97</t>
-  </si>
-  <si>
-    <t>penis</t>
-  </si>
-  <si>
-    <t>46dc363a5e754c6781f8889094b288c4</t>
   </si>
 </sst>
 </file>
@@ -360,42 +348,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:B5"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B1" t="s">
         <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>123</v>
-      </c>
-      <c r="B3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>